<commit_message>
Reran Sonoran 4.1.R in case any species info changed; had some weird manual edits I had to do to edited3 (regarding UNFO-1.SRER and UNFO-2.SRER being switched, and also something with BORA/BOCUspp rows, and I don't know how those problems were created, but it's fine now
</commit_message>
<xml_diff>
--- a/Sonoran-data/data-wrangling-intermediate/04.1b_edited1_corrected-seeded-in-mix_subplot.xlsx
+++ b/Sonoran-data/data-wrangling-intermediate/04.1b_edited1_corrected-seeded-in-mix_subplot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/Sonoran-data/data-wrangling-intermediate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eltnmsu-my.sharepoint.com/personal/lossanna_nmsu_edu/Documents/Documents/02_RestoreNet/RestoreNet/Sonoran-data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="13_ncr:40009_{28A3A110-A06D-4DF3-ACB9-0ADAC0A6265D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{937DE7CF-A8FF-42C7-B2E6-3E4077664D41}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:40009_{28A3A110-A06D-4DF3-ACB9-0ADAC0A6265D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE3A0EFA-EC6B-4D70-814D-EF8C148D4EBF}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -239,7 +239,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,6 +373,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="35">
@@ -728,10 +734,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -800,8 +807,8 @@
       <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>592455</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
@@ -819,7 +826,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9132570" y="281940"/>
-          <a:ext cx="2562225" cy="2964180"/>
+          <a:ext cx="2975610" cy="2964180"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -854,16 +861,46 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
             <a:t>Corrected according to</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> `with-site` tab from `from-Master_seed-mix_LO.xlsx`.</a:t>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>with-site</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> tab from </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>from-Master_seed-mix_LO.xlsx</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>.</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
+            <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
@@ -884,7 +921,9 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
             <a:t>Yellow highlighting indicates SpeciesSeeded value was changed. Usually </a:t>
           </a:r>
           <a:r>
@@ -893,26 +932,34 @@
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
               <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>discrepancies</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
             <a:t> are because the PlotMix column is conflicting (species weren't included in both warm and cool mixes, so there can only be one for any of them per site).</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
+            <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
             <a:t>Green highlighting indicates SpeciesSeeded column was changed to be standardized in "Yes" format.</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:latin typeface="Aptos Narrow" panose="020B0004020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1221,8 +1268,8 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1237,2498 +1284,2498 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="G4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="G5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="I5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="G6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="G7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="G8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="I8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="G9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="1" t="s">
+      <c r="I9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="G10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="I10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="G11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I11" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="I11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="G12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="I12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="G13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="I13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="B14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="G14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" s="1" t="s">
+      <c r="I14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G15" t="s">
-        <v>6</v>
-      </c>
-      <c r="H15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" t="s">
-        <v>14</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="G15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G16" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" t="s">
-        <v>14</v>
-      </c>
-      <c r="J16" s="1" t="s">
+      <c r="G16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" t="s">
-        <v>14</v>
-      </c>
-      <c r="J17" s="1" t="s">
+      <c r="G17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G18" t="s">
-        <v>6</v>
-      </c>
-      <c r="H18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" t="s">
+      <c r="G18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H19" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" t="s">
+      <c r="G19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G20" t="s">
-        <v>6</v>
-      </c>
-      <c r="H20" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="G20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="G21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I21" t="s">
-        <v>14</v>
-      </c>
-      <c r="J21" t="s">
+      <c r="I21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G22" t="s">
-        <v>6</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="G22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G23" t="s">
-        <v>6</v>
-      </c>
-      <c r="H23" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="G23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G24" t="s">
-        <v>6</v>
-      </c>
-      <c r="H24" t="s">
-        <v>17</v>
-      </c>
-      <c r="I24" t="s">
+      <c r="G24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G25" t="s">
-        <v>6</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="G25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I25" t="s">
-        <v>14</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="I25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="B26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G26" t="s">
-        <v>6</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="G26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I26" t="s">
-        <v>14</v>
-      </c>
-      <c r="J26" s="1" t="s">
+      <c r="I26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="B27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G27" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="G27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I27" t="s">
-        <v>14</v>
-      </c>
-      <c r="J27" s="1" t="s">
+      <c r="I27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B28" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G28" t="s">
-        <v>6</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="G28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I28" t="s">
-        <v>14</v>
-      </c>
-      <c r="J28" t="s">
+      <c r="I28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B29" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G29" t="s">
-        <v>6</v>
-      </c>
-      <c r="H29" t="s">
+      <c r="G29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I29" t="s">
-        <v>14</v>
-      </c>
-      <c r="J29" t="s">
+      <c r="I29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="B30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G30" t="s">
-        <v>6</v>
-      </c>
-      <c r="H30" t="s">
+      <c r="G30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I30" t="s">
-        <v>14</v>
-      </c>
-      <c r="J30" s="1" t="s">
+      <c r="I30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="B31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G31" t="s">
-        <v>6</v>
-      </c>
-      <c r="H31" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" t="s">
-        <v>14</v>
-      </c>
-      <c r="J31" t="s">
+      <c r="G31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B32" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G32" t="s">
-        <v>6</v>
-      </c>
-      <c r="H32" t="s">
-        <v>17</v>
-      </c>
-      <c r="I32" t="s">
-        <v>14</v>
-      </c>
-      <c r="J32" t="s">
+      <c r="G32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B33" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="B33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G33" t="s">
-        <v>6</v>
-      </c>
-      <c r="H33" t="s">
-        <v>17</v>
-      </c>
-      <c r="I33" t="s">
+      <c r="G33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J33" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B34" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="B34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G34" t="s">
-        <v>6</v>
-      </c>
-      <c r="H34" t="s">
-        <v>17</v>
-      </c>
-      <c r="I34" t="s">
+      <c r="G34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J34" t="s">
+      <c r="J34" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B35" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G35" t="s">
-        <v>6</v>
-      </c>
-      <c r="H35" t="s">
+      <c r="G35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I35" t="s">
-        <v>14</v>
-      </c>
-      <c r="J35" t="s">
+      <c r="I35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B36" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="B36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G36" t="s">
-        <v>6</v>
-      </c>
-      <c r="H36" t="s">
-        <v>17</v>
-      </c>
-      <c r="I36" t="s">
+      <c r="G36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J36" t="s">
+      <c r="J36" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B37" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="B37" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G37" t="s">
-        <v>6</v>
-      </c>
-      <c r="H37" t="s">
-        <v>17</v>
-      </c>
-      <c r="I37" t="s">
+      <c r="G37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="J37" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B38" t="s">
-        <v>44</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="B38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G38" t="s">
-        <v>6</v>
-      </c>
-      <c r="H38" t="s">
+      <c r="G38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I38" t="s">
-        <v>14</v>
-      </c>
-      <c r="J38" t="s">
+      <c r="I38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J38" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B39" t="s">
-        <v>44</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="B39" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G39" t="s">
-        <v>6</v>
-      </c>
-      <c r="H39" t="s">
+      <c r="G39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I39" t="s">
-        <v>14</v>
-      </c>
-      <c r="J39" s="1" t="s">
+      <c r="I39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J39" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B40" t="s">
-        <v>44</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="B40" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G40" t="s">
-        <v>6</v>
-      </c>
-      <c r="H40" t="s">
+      <c r="G40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I40" t="s">
-        <v>14</v>
-      </c>
-      <c r="J40" t="s">
+      <c r="I40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B41" t="s">
-        <v>44</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="B41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G41" t="s">
-        <v>6</v>
-      </c>
-      <c r="H41" t="s">
+      <c r="G41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I41" t="s">
-        <v>14</v>
-      </c>
-      <c r="J41" t="s">
+      <c r="I41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J41" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B42" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="B42" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G42" t="s">
-        <v>6</v>
-      </c>
-      <c r="H42" t="s">
+      <c r="G42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I42" t="s">
-        <v>14</v>
-      </c>
-      <c r="J42" s="1" t="s">
+      <c r="I42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B43" t="s">
-        <v>44</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="B43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G43" t="s">
-        <v>6</v>
-      </c>
-      <c r="H43" t="s">
-        <v>17</v>
-      </c>
-      <c r="I43" t="s">
-        <v>14</v>
-      </c>
-      <c r="J43" t="s">
+      <c r="G43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J43" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B44" t="s">
-        <v>44</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="B44" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G44" t="s">
-        <v>6</v>
-      </c>
-      <c r="H44" t="s">
-        <v>17</v>
-      </c>
-      <c r="I44" t="s">
-        <v>14</v>
-      </c>
-      <c r="J44" t="s">
+      <c r="G44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J44" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="A45" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B45" t="s">
-        <v>44</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="B45" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G45" t="s">
-        <v>6</v>
-      </c>
-      <c r="H45" t="s">
-        <v>17</v>
-      </c>
-      <c r="I45" t="s">
-        <v>14</v>
-      </c>
-      <c r="J45" s="1" t="s">
+      <c r="G45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J45" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="A46" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B46" t="s">
-        <v>44</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="B46" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G46" t="s">
-        <v>6</v>
-      </c>
-      <c r="H46" t="s">
-        <v>17</v>
-      </c>
-      <c r="I46" t="s">
+      <c r="G46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I46" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J46" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="A47" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B47" t="s">
-        <v>44</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="B47" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G47" t="s">
-        <v>6</v>
-      </c>
-      <c r="H47" t="s">
-        <v>17</v>
-      </c>
-      <c r="I47" t="s">
+      <c r="G47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I47" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J47" t="s">
+      <c r="J47" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="A48" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B48" t="s">
-        <v>44</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="B48" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G48" t="s">
-        <v>6</v>
-      </c>
-      <c r="H48" t="s">
-        <v>17</v>
-      </c>
-      <c r="I48" t="s">
+      <c r="G48" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J48" t="s">
+      <c r="J48" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="A49" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B49" t="s">
-        <v>44</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="B49" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G49" t="s">
-        <v>6</v>
-      </c>
-      <c r="H49" t="s">
+      <c r="G49" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I49" t="s">
-        <v>14</v>
-      </c>
-      <c r="J49" t="s">
+      <c r="I49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J49" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="A50" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B50" t="s">
-        <v>44</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="B50" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G50" t="s">
-        <v>6</v>
-      </c>
-      <c r="H50" t="s">
-        <v>17</v>
-      </c>
-      <c r="I50" t="s">
+      <c r="G50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I50" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J50" t="s">
+      <c r="J50" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="A51" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B51" t="s">
-        <v>44</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="B51" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G51" t="s">
-        <v>6</v>
-      </c>
-      <c r="H51" t="s">
+      <c r="G51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H51" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I51" t="s">
-        <v>14</v>
-      </c>
-      <c r="J51" t="s">
+      <c r="I51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J51" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="A52" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B52" t="s">
-        <v>44</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="B52" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G52" t="s">
-        <v>6</v>
-      </c>
-      <c r="H52" t="s">
+      <c r="G52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I52" t="s">
-        <v>14</v>
-      </c>
-      <c r="J52" t="s">
+      <c r="I52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J52" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="A53" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B53" t="s">
-        <v>44</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="B53" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G53" t="s">
-        <v>6</v>
-      </c>
-      <c r="H53" t="s">
-        <v>17</v>
-      </c>
-      <c r="I53" t="s">
-        <v>14</v>
-      </c>
-      <c r="J53" t="s">
+      <c r="G53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J53" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="A54" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G54" t="s">
-        <v>6</v>
-      </c>
-      <c r="H54" t="s">
-        <v>17</v>
-      </c>
-      <c r="I54" t="s">
+      <c r="G54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I54" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J54" t="s">
+      <c r="J54" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="A55" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G55" t="s">
-        <v>6</v>
-      </c>
-      <c r="H55" t="s">
-        <v>17</v>
-      </c>
-      <c r="I55" t="s">
+      <c r="G55" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I55" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J55" s="2" t="s">
+      <c r="J55" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+      <c r="A56" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G56" t="s">
-        <v>6</v>
-      </c>
-      <c r="H56" t="s">
-        <v>17</v>
-      </c>
-      <c r="I56" t="s">
-        <v>14</v>
-      </c>
-      <c r="J56" t="s">
+      <c r="G56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J56" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+      <c r="A57" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G57" t="s">
-        <v>6</v>
-      </c>
-      <c r="H57" t="s">
+      <c r="G57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I57" t="s">
-        <v>14</v>
-      </c>
-      <c r="J57" t="s">
+      <c r="I57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J57" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+      <c r="A58" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E58" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="F58" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G58" t="s">
-        <v>6</v>
-      </c>
-      <c r="H58" t="s">
+      <c r="G58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H58" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I58" t="s">
-        <v>14</v>
-      </c>
-      <c r="J58" s="1" t="s">
+      <c r="I58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J58" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="A59" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G59" t="s">
-        <v>6</v>
-      </c>
-      <c r="H59" t="s">
-        <v>17</v>
-      </c>
-      <c r="I59" t="s">
+      <c r="G59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I59" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J59" t="s">
+      <c r="J59" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+      <c r="A60" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G60" t="s">
-        <v>6</v>
-      </c>
-      <c r="H60" t="s">
-        <v>17</v>
-      </c>
-      <c r="I60" t="s">
+      <c r="G60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I60" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J60" t="s">
+      <c r="J60" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="A61" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G61" t="s">
-        <v>6</v>
-      </c>
-      <c r="H61" t="s">
+      <c r="G61" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H61" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I61" t="s">
-        <v>14</v>
-      </c>
-      <c r="J61" t="s">
+      <c r="I61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J61" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+      <c r="A62" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G62" t="s">
-        <v>6</v>
-      </c>
-      <c r="H62" t="s">
-        <v>17</v>
-      </c>
-      <c r="I62" t="s">
+      <c r="G62" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I62" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J62" t="s">
+      <c r="J62" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+      <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G63" t="s">
-        <v>6</v>
-      </c>
-      <c r="H63" t="s">
-        <v>17</v>
-      </c>
-      <c r="I63" t="s">
-        <v>14</v>
-      </c>
-      <c r="J63" t="s">
+      <c r="G63" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J63" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+      <c r="A64" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G64" t="s">
-        <v>6</v>
-      </c>
-      <c r="H64" t="s">
-        <v>17</v>
-      </c>
-      <c r="I64" t="s">
-        <v>14</v>
-      </c>
-      <c r="J64" s="2" t="s">
+      <c r="G64" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J64" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+      <c r="A65" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G65" t="s">
-        <v>6</v>
-      </c>
-      <c r="H65" t="s">
-        <v>17</v>
-      </c>
-      <c r="I65" t="s">
-        <v>14</v>
-      </c>
-      <c r="J65" s="2" t="s">
+      <c r="G65" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J65" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+      <c r="A66" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G66" t="s">
-        <v>6</v>
-      </c>
-      <c r="H66" t="s">
-        <v>17</v>
-      </c>
-      <c r="I66" t="s">
+      <c r="G66" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I66" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J66" t="s">
+      <c r="J66" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+      <c r="A67" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G67" t="s">
-        <v>6</v>
-      </c>
-      <c r="H67" t="s">
-        <v>17</v>
-      </c>
-      <c r="I67" t="s">
+      <c r="G67" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I67" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J67" s="2" t="s">
+      <c r="J67" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+      <c r="A68" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G68" t="s">
-        <v>6</v>
-      </c>
-      <c r="H68" t="s">
-        <v>17</v>
-      </c>
-      <c r="I68" t="s">
+      <c r="G68" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I68" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J68" t="s">
+      <c r="J68" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+      <c r="A69" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G69" t="s">
-        <v>6</v>
-      </c>
-      <c r="H69" t="s">
-        <v>17</v>
-      </c>
-      <c r="I69" t="s">
+      <c r="G69" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I69" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J69" s="2" t="s">
+      <c r="J69" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+      <c r="A70" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F70" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G70" t="s">
-        <v>6</v>
-      </c>
-      <c r="H70" t="s">
-        <v>17</v>
-      </c>
-      <c r="I70" t="s">
-        <v>14</v>
-      </c>
-      <c r="J70" s="2" t="s">
+      <c r="G70" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J70" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+      <c r="A71" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F71" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G71" t="s">
-        <v>6</v>
-      </c>
-      <c r="H71" t="s">
-        <v>17</v>
-      </c>
-      <c r="I71" t="s">
+      <c r="G71" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I71" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J71" t="s">
+      <c r="J71" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+      <c r="A72" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D72" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="E72" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F72" s="1" t="s">
+      <c r="F72" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G72" t="s">
-        <v>6</v>
-      </c>
-      <c r="H72" t="s">
-        <v>17</v>
-      </c>
-      <c r="I72" t="s">
+      <c r="G72" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I72" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J72" s="1" t="s">
+      <c r="J72" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+      <c r="A73" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="E73" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F73" s="1" t="s">
+      <c r="F73" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G73" t="s">
-        <v>6</v>
-      </c>
-      <c r="H73" t="s">
-        <v>17</v>
-      </c>
-      <c r="I73" t="s">
+      <c r="G73" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I73" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J73" s="1" t="s">
+      <c r="J73" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+      <c r="A74" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D74" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="E74" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F74" s="1" t="s">
+      <c r="F74" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G74" t="s">
-        <v>6</v>
-      </c>
-      <c r="H74" t="s">
-        <v>17</v>
-      </c>
-      <c r="I74" t="s">
+      <c r="G74" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I74" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J74" s="1" t="s">
+      <c r="J74" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+      <c r="A75" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F75" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G75" t="s">
-        <v>6</v>
-      </c>
-      <c r="H75" t="s">
-        <v>17</v>
-      </c>
-      <c r="I75" t="s">
+      <c r="G75" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I75" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J75" t="s">
+      <c r="J75" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+      <c r="A76" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G76" t="s">
-        <v>6</v>
-      </c>
-      <c r="H76" t="s">
+      <c r="G76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H76" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I76" t="s">
-        <v>14</v>
-      </c>
-      <c r="J76" t="s">
+      <c r="I76" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J76" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+      <c r="A77" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F77" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G77" t="s">
-        <v>6</v>
-      </c>
-      <c r="H77" t="s">
-        <v>17</v>
-      </c>
-      <c r="I77" t="s">
-        <v>14</v>
-      </c>
-      <c r="J77" s="2" t="s">
+      <c r="G77" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J77" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+      <c r="A78" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G78" t="s">
-        <v>6</v>
-      </c>
-      <c r="H78" t="s">
-        <v>17</v>
-      </c>
-      <c r="I78" t="s">
-        <v>14</v>
-      </c>
-      <c r="J78" t="s">
+      <c r="G78" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J78" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>